<commit_message>
add query and text
</commit_message>
<xml_diff>
--- a/cmd/Список аварий.xlsx
+++ b/cmd/Список аварий.xlsx
@@ -1,20 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="true" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+  <si>
+    <t>2009-08-08</t>
+  </si>
+  <si>
+    <t>Jgbcyf</t>
+  </si>
+  <si>
+    <t>2008-07-09</t>
+  </si>
+  <si>
+    <t>Описание ошибки</t>
+  </si>
   <si>
     <t>2003-01-01</t>
   </si>
@@ -25,16 +37,58 @@
     <t>2001-01-01</t>
   </si>
   <si>
+    <t>Ошибка главного контроллера</t>
+  </si>
+  <si>
     <t>Ошибка чегото чегото</t>
   </si>
   <si>
+    <t>2009-04-05</t>
+  </si>
+  <si>
+    <t>aljhgqalf</t>
+  </si>
+  <si>
+    <t>2008-09-09</t>
+  </si>
+  <si>
+    <t>2008-04-05</t>
+  </si>
+  <si>
+    <t>Описание ошибки рррр</t>
+  </si>
+  <si>
     <t>Ошибка ошибка ошибка</t>
+  </si>
+  <si>
+    <t>2024-01-06</t>
+  </si>
+  <si>
+    <t>gjdgfxbg</t>
+  </si>
+  <si>
+    <t>jgbcyfb ороплы лдоцке</t>
+  </si>
+  <si>
+    <t>2008-09-05</t>
+  </si>
+  <si>
+    <t>2001-05-07</t>
+  </si>
+  <si>
+    <t>Ошибкак главного вала выскокая темепратруа</t>
+  </si>
+  <si>
+    <t>2099-01-01</t>
+  </si>
+  <si>
+    <t>fsdghsh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -67,15 +121,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -117,7 +171,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -152,7 +206,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -332,13 +386,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="42.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4">
       <c r="A1">
         <v>12</v>
       </c>
@@ -346,13 +408,13 @@
         <v>0</v>
       </c>
       <c r="C1">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>12</v>
       </c>
@@ -360,26 +422,181 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>123</v>
+        <v>321</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4">
       <c r="A3">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>345</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>123</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>123</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>453</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>123</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>2222</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>245</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>314</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>134</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>442</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>425</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>555</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>345</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add test for controllers, excel
</commit_message>
<xml_diff>
--- a/cmd/Список аварий.xlsx
+++ b/cmd/Список аварий.xlsx
@@ -1,94 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="true" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>2009-08-08</t>
+    <t>2000-01-01</t>
   </si>
   <si>
-    <t>Jgbcyf</t>
-  </si>
-  <si>
-    <t>2008-07-09</t>
-  </si>
-  <si>
-    <t>Описание ошибки</t>
-  </si>
-  <si>
-    <t>2003-01-01</t>
-  </si>
-  <si>
-    <t>Ошибка энкодера поворота лопасти</t>
-  </si>
-  <si>
-    <t>2001-01-01</t>
-  </si>
-  <si>
-    <t>Ошибка главного контроллера</t>
-  </si>
-  <si>
-    <t>Ошибка чегото чегото</t>
-  </si>
-  <si>
-    <t>2009-04-05</t>
-  </si>
-  <si>
-    <t>aljhgqalf</t>
-  </si>
-  <si>
-    <t>2008-09-09</t>
-  </si>
-  <si>
-    <t>2008-04-05</t>
-  </si>
-  <si>
-    <t>Описание ошибки рррр</t>
-  </si>
-  <si>
-    <t>Ошибка ошибка ошибка</t>
-  </si>
-  <si>
-    <t>2024-01-06</t>
-  </si>
-  <si>
-    <t>gjdgfxbg</t>
-  </si>
-  <si>
-    <t>jgbcyfb ороплы лдоцке</t>
-  </si>
-  <si>
-    <t>2008-09-05</t>
-  </si>
-  <si>
-    <t>2001-05-07</t>
-  </si>
-  <si>
-    <t>Ошибкак главного вала выскокая темепратруа</t>
-  </si>
-  <si>
-    <t>2099-01-01</t>
-  </si>
-  <si>
-    <t>fsdghsh</t>
+    <t>Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -121,15 +58,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -171,7 +108,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -206,7 +143,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -386,217 +323,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
+    <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="42.109375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1">
       <c r="A1">
-        <v>12</v>
+        <v>555</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1">
-        <v>12</v>
+        <v>555</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2">
       <c r="A2">
-        <v>12</v>
+        <v>555</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>321</v>
+        <v>555</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3">
-        <v>12</v>
+        <v>555</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>123</v>
+        <v>555</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4">
-        <v>12</v>
+        <v>555</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>345</v>
+        <v>555</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5">
-        <v>12</v>
+        <v>555</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>123</v>
+        <v>555</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6">
-        <v>22</v>
+        <v>555</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>123</v>
+        <v>555</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7">
-        <v>22</v>
+        <v>555</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>44</v>
+        <v>555</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8">
-        <v>22</v>
+        <v>555</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>453</v>
+        <v>555</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>123</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>2222</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10">
-        <v>245</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>314</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12">
-        <v>134</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>442</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13">
-        <v>425</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>555</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14">
-        <v>345</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>